<commit_message>
refactored words into objects
</commit_message>
<xml_diff>
--- a/otmazy_words.xlsx
+++ b/otmazy_words.xlsx
@@ -3,11 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="spice" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="subj" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="glagol" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="predlog" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="context" sheetId="5" r:id="rId8"/>
+    <sheet state="hidden" name="subj" sheetId="1" r:id="rId4"/>
+    <sheet state="hidden" name="glagol" sheetId="2" r:id="rId5"/>
+    <sheet state="hidden" name="predlog" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="context" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="beginning" sheetId="5" r:id="rId8"/>
     <sheet state="visible" name="noun" sheetId="6" r:id="rId9"/>
     <sheet state="visible" name="verb" sheetId="7" r:id="rId10"/>
     <sheet state="hidden" name="слова v1" sheetId="8" r:id="rId11"/>
@@ -18,323 +18,356 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="246">
   <si>
     <t>id</t>
   </si>
   <si>
+    <t>predlog</t>
+  </si>
+  <si>
     <t>glagol</t>
   </si>
   <si>
     <t>субъект</t>
   </si>
   <si>
+    <t>object</t>
+  </si>
+  <si>
+    <t>тип субъекта</t>
+  </si>
+  <si>
+    <t>destination</t>
+  </si>
+  <si>
+    <t>начало</t>
+  </si>
+  <si>
+    <t>event</t>
+  </si>
+  <si>
+    <t>inanimate_obj</t>
+  </si>
+  <si>
+    <t>animate_obj</t>
+  </si>
+  <si>
+    <t>movable_obj</t>
+  </si>
+  <si>
+    <t>sklonenie_object</t>
+  </si>
+  <si>
+    <t>sklonenie_destination</t>
+  </si>
+  <si>
+    <t>склонение_место</t>
+  </si>
+  <si>
+    <t>к</t>
+  </si>
+  <si>
+    <t>в</t>
+  </si>
+  <si>
+    <t>из</t>
+  </si>
+  <si>
+    <t>от</t>
+  </si>
+  <si>
+    <t>на</t>
+  </si>
+  <si>
+    <t>о</t>
+  </si>
+  <si>
+    <t>везти</t>
+  </si>
+  <si>
+    <t>accs</t>
+  </si>
+  <si>
+    <t>вести</t>
+  </si>
+  <si>
+    <t>забрать</t>
+  </si>
+  <si>
+    <t>отвезти</t>
+  </si>
+  <si>
+    <t>отвести</t>
+  </si>
+  <si>
+    <t>принести</t>
+  </si>
+  <si>
+    <t>отнести</t>
+  </si>
+  <si>
+    <t>сдать</t>
+  </si>
+  <si>
+    <t>отправить</t>
+  </si>
+  <si>
+    <t>убрать</t>
+  </si>
+  <si>
+    <t>сходить</t>
+  </si>
+  <si>
+    <t>loc2</t>
+  </si>
+  <si>
+    <t>убраться</t>
+  </si>
+  <si>
+    <t>loct</t>
+  </si>
+  <si>
+    <t>прийти</t>
+  </si>
+  <si>
+    <t>позаботиться о</t>
+  </si>
+  <si>
+    <t>решить вопрос с</t>
+  </si>
+  <si>
+    <t>ablt</t>
+  </si>
+  <si>
+    <t>уехать</t>
+  </si>
+  <si>
+    <t>отремонтировать</t>
+  </si>
+  <si>
+    <t>доделать</t>
+  </si>
+  <si>
+    <t>подбросить</t>
+  </si>
+  <si>
+    <t>создать</t>
+  </si>
+  <si>
+    <t>склепать</t>
+  </si>
+  <si>
+    <t>забабахать</t>
+  </si>
+  <si>
+    <t>заебенить</t>
+  </si>
+  <si>
+    <t>сделать</t>
+  </si>
+  <si>
+    <t>довезти</t>
+  </si>
+  <si>
+    <t>довести</t>
+  </si>
+  <si>
+    <t>я</t>
+  </si>
+  <si>
+    <t>допереть</t>
+  </si>
+  <si>
+    <t>должен</t>
+  </si>
+  <si>
+    <t>обдумать</t>
+  </si>
+  <si>
+    <t>собираюсь</t>
+  </si>
+  <si>
+    <t>подумать о</t>
+  </si>
+  <si>
+    <t>обещал</t>
+  </si>
+  <si>
+    <t>хотел</t>
+  </si>
+  <si>
+    <t>запланировать</t>
+  </si>
+  <si>
+    <t>буду</t>
+  </si>
+  <si>
+    <t>давно собираюсь</t>
+  </si>
+  <si>
+    <t>давно обещал</t>
+  </si>
+  <si>
+    <t>очень хотел</t>
+  </si>
+  <si>
+    <t>давно хотел</t>
+  </si>
+  <si>
+    <t>точно буду</t>
+  </si>
+  <si>
+    <t>мне</t>
+  </si>
+  <si>
+    <t>надо</t>
+  </si>
+  <si>
+    <t>контекст</t>
+  </si>
+  <si>
+    <t>работа</t>
+  </si>
+  <si>
+    <t>очень надо</t>
+  </si>
+  <si>
+    <t>семья</t>
+  </si>
+  <si>
+    <t>придется</t>
+  </si>
+  <si>
+    <t>друзья</t>
+  </si>
+  <si>
+    <t>точно придется</t>
+  </si>
+  <si>
+    <t>пора</t>
+  </si>
+  <si>
+    <t>давно пора</t>
+  </si>
+  <si>
+    <t>очень давно пора</t>
+  </si>
+  <si>
+    <t>стоит</t>
+  </si>
+  <si>
+    <t>давно стоит</t>
+  </si>
+  <si>
+    <t>явно придется</t>
+  </si>
+  <si>
+    <t>явно стоит</t>
+  </si>
+  <si>
+    <t>явно надо</t>
+  </si>
+  <si>
+    <t>страшно надо</t>
+  </si>
+  <si>
+    <t>критически важно</t>
+  </si>
+  <si>
+    <t>очень важно</t>
+  </si>
+  <si>
     <t>спайс</t>
   </si>
   <si>
-    <t>object</t>
-  </si>
-  <si>
-    <t>тип субъекта</t>
-  </si>
-  <si>
-    <t>destination</t>
-  </si>
-  <si>
-    <t>начало</t>
-  </si>
-  <si>
-    <t>event</t>
-  </si>
-  <si>
-    <t>inanimate_obj</t>
-  </si>
-  <si>
-    <t>animate_obj</t>
-  </si>
-  <si>
-    <t>movable_obj</t>
-  </si>
-  <si>
-    <t>sklonenie_object</t>
-  </si>
-  <si>
-    <t>sklonenie_destination</t>
-  </si>
-  <si>
-    <t>склонение_место</t>
+    <t>comma_after</t>
+  </si>
+  <si>
+    <t>tense</t>
   </si>
   <si>
     <t>извини</t>
   </si>
   <si>
-    <t>я</t>
-  </si>
-  <si>
-    <t>везти</t>
+    <t>all</t>
   </si>
   <si>
     <t>увы</t>
   </si>
   <si>
-    <t>должен</t>
-  </si>
-  <si>
     <t>к сожалению</t>
   </si>
   <si>
-    <t>accs</t>
+    <t>future</t>
   </si>
   <si>
     <t>эх</t>
   </si>
   <si>
-    <t>вести</t>
-  </si>
-  <si>
-    <t>собираюсь</t>
-  </si>
-  <si>
     <t>сорян</t>
   </si>
   <si>
     <t>блин</t>
   </si>
   <si>
-    <t>обещал</t>
-  </si>
-  <si>
     <t>вот чёрт</t>
   </si>
   <si>
-    <t>хотел</t>
-  </si>
-  <si>
-    <t>забрать</t>
+    <t>noun</t>
+  </si>
+  <si>
+    <t>obj</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>type</t>
   </si>
   <si>
     <t>совсем забыл</t>
   </si>
   <si>
-    <t>буду</t>
+    <t>type_alt</t>
   </si>
   <si>
     <t>я бы с радостью, но</t>
   </si>
   <si>
-    <t>давно собираюсь</t>
-  </si>
-  <si>
-    <t>отвезти</t>
-  </si>
-  <si>
-    <t>давно обещал</t>
-  </si>
-  <si>
     <t>чёрт</t>
   </si>
   <si>
-    <t>очень хотел</t>
-  </si>
-  <si>
-    <t>отвести</t>
-  </si>
-  <si>
-    <t>давно хотел</t>
-  </si>
-  <si>
-    <t>точно буду</t>
-  </si>
-  <si>
-    <t>мне</t>
-  </si>
-  <si>
-    <t>принести</t>
-  </si>
-  <si>
-    <t>надо</t>
-  </si>
-  <si>
-    <t>очень надо</t>
-  </si>
-  <si>
-    <t>отнести</t>
-  </si>
-  <si>
-    <t>придется</t>
-  </si>
-  <si>
-    <t>сдать</t>
-  </si>
-  <si>
-    <t>точно придется</t>
-  </si>
-  <si>
-    <t>пора</t>
-  </si>
-  <si>
-    <t>отправить</t>
-  </si>
-  <si>
-    <t>давно пора</t>
-  </si>
-  <si>
-    <t>очень давно пора</t>
-  </si>
-  <si>
-    <t>убрать</t>
-  </si>
-  <si>
-    <t>стоит</t>
-  </si>
-  <si>
-    <t>сходить</t>
-  </si>
-  <si>
-    <t>давно стоит</t>
-  </si>
-  <si>
-    <t>loc2</t>
-  </si>
-  <si>
-    <t>явно придется</t>
-  </si>
-  <si>
-    <t>убраться</t>
-  </si>
-  <si>
-    <t>явно стоит</t>
-  </si>
-  <si>
-    <t>loct</t>
-  </si>
-  <si>
-    <t>прийти</t>
-  </si>
-  <si>
-    <t>явно надо</t>
-  </si>
-  <si>
-    <t>страшно надо</t>
-  </si>
-  <si>
-    <t>позаботиться о</t>
-  </si>
-  <si>
-    <t>критически важно</t>
-  </si>
-  <si>
-    <t>очень важно</t>
-  </si>
-  <si>
-    <t>решить вопрос с</t>
-  </si>
-  <si>
-    <t>ablt</t>
-  </si>
-  <si>
-    <t>уехать</t>
-  </si>
-  <si>
-    <t>отремонтировать</t>
-  </si>
-  <si>
-    <t>доделать</t>
-  </si>
-  <si>
-    <t>подбросить</t>
-  </si>
-  <si>
-    <t>создать</t>
-  </si>
-  <si>
-    <t>predlog</t>
-  </si>
-  <si>
-    <t>к</t>
-  </si>
-  <si>
-    <t>склепать</t>
-  </si>
-  <si>
-    <t>в</t>
-  </si>
-  <si>
-    <t>забабахать</t>
-  </si>
-  <si>
-    <t>из</t>
-  </si>
-  <si>
-    <t>от</t>
-  </si>
-  <si>
-    <t>на</t>
-  </si>
-  <si>
-    <t>заебенить</t>
-  </si>
-  <si>
-    <t>о</t>
-  </si>
-  <si>
-    <t>сделать</t>
-  </si>
-  <si>
-    <t>довезти</t>
-  </si>
-  <si>
-    <t>довести</t>
-  </si>
-  <si>
-    <t>допереть</t>
-  </si>
-  <si>
-    <t>обдумать</t>
-  </si>
-  <si>
-    <t>подумать о</t>
-  </si>
-  <si>
-    <t>запланировать</t>
-  </si>
-  <si>
-    <t>контекст</t>
-  </si>
-  <si>
-    <t>работа</t>
-  </si>
-  <si>
-    <t>семья</t>
-  </si>
-  <si>
-    <t>друзья</t>
-  </si>
-  <si>
-    <t>noun</t>
-  </si>
-  <si>
-    <t>obj</t>
-  </si>
-  <si>
-    <t>target</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>type_alt</t>
-  </si>
-  <si>
     <t>predlog_if_obst</t>
   </si>
   <si>
+    <t>только что понял</t>
+  </si>
+  <si>
+    <t>noun_type</t>
+  </si>
+  <si>
+    <t>noun_type_alt</t>
+  </si>
+  <si>
     <t>собака</t>
   </si>
   <si>
+    <t>to_be</t>
+  </si>
+  <si>
+    <t>как раз</t>
+  </si>
+  <si>
+    <t>move</t>
+  </si>
+  <si>
     <t>thing</t>
   </si>
   <si>
+    <t>бляха-муха</t>
+  </si>
+  <si>
     <t>кошка</t>
   </si>
   <si>
@@ -344,334 +377,385 @@
     <t>person</t>
   </si>
   <si>
+    <t>ребенок</t>
+  </si>
+  <si>
+    <t>дети</t>
+  </si>
+  <si>
+    <t>remove</t>
+  </si>
+  <si>
+    <t>дочь</t>
+  </si>
+  <si>
+    <t>сын</t>
+  </si>
+  <si>
+    <t>друг</t>
+  </si>
+  <si>
+    <t>подруга</t>
+  </si>
+  <si>
+    <t>отец</t>
+  </si>
+  <si>
+    <t>мать</t>
+  </si>
+  <si>
+    <t>квартира</t>
+  </si>
+  <si>
+    <t>place</t>
+  </si>
+  <si>
+    <t>дом</t>
+  </si>
+  <si>
+    <t>кухня</t>
+  </si>
+  <si>
+    <t>place_open</t>
+  </si>
+  <si>
+    <t>travel</t>
+  </si>
+  <si>
+    <t>goal</t>
+  </si>
+  <si>
+    <t>ванная</t>
+  </si>
+  <si>
+    <t>позаботиться</t>
+  </si>
+  <si>
+    <t>унитаз</t>
+  </si>
+  <si>
+    <t>решить</t>
+  </si>
+  <si>
+    <t>ноутбук</t>
+  </si>
+  <si>
+    <t>телефон</t>
+  </si>
+  <si>
+    <t>смартфон</t>
+  </si>
+  <si>
+    <t>документы</t>
+  </si>
+  <si>
+    <t>тёща</t>
+  </si>
+  <si>
+    <t>project</t>
+  </si>
+  <si>
+    <t>тесть</t>
+  </si>
+  <si>
+    <t>свекровь</t>
+  </si>
+  <si>
+    <t>свёкр</t>
+  </si>
+  <si>
+    <t>бабушка</t>
+  </si>
+  <si>
+    <t>дедушка</t>
+  </si>
+  <si>
+    <t>дядя</t>
+  </si>
+  <si>
+    <t>вот жалость</t>
+  </si>
+  <si>
+    <t>тётя</t>
+  </si>
+  <si>
+    <t>ковёр</t>
+  </si>
+  <si>
+    <t>фикус</t>
+  </si>
+  <si>
+    <t>кактус</t>
+  </si>
+  <si>
+    <t>мебель</t>
+  </si>
+  <si>
+    <t>подумать</t>
+  </si>
+  <si>
+    <t>телек</t>
+  </si>
+  <si>
+    <t>ноут</t>
+  </si>
+  <si>
+    <t>убирать</t>
+  </si>
+  <si>
+    <t>автомастерская</t>
+  </si>
+  <si>
+    <t>добраться</t>
+  </si>
+  <si>
+    <t>ремонт</t>
+  </si>
+  <si>
+    <t>выбраться</t>
+  </si>
+  <si>
+    <t>обучение</t>
+  </si>
+  <si>
+    <t>гипермаркет</t>
+  </si>
+  <si>
+    <t>зайти</t>
+  </si>
+  <si>
+    <t>ЖЭК</t>
+  </si>
+  <si>
+    <t>забежать</t>
+  </si>
+  <si>
+    <t>нотариус</t>
+  </si>
+  <si>
+    <t>съездить</t>
+  </si>
+  <si>
+    <t>врач</t>
+  </si>
+  <si>
+    <t>доктор</t>
+  </si>
+  <si>
+    <t>поехать</t>
+  </si>
+  <si>
+    <t>центр госуслуг</t>
+  </si>
+  <si>
+    <t>курсы</t>
+  </si>
+  <si>
+    <t>совещание</t>
+  </si>
+  <si>
+    <t>родственники</t>
+  </si>
+  <si>
+    <t>сгонять</t>
+  </si>
+  <si>
+    <t>дача</t>
+  </si>
+  <si>
+    <t>хранение</t>
+  </si>
+  <si>
+    <t>банк</t>
+  </si>
+  <si>
+    <t>планерка</t>
+  </si>
+  <si>
+    <t>свадьба</t>
+  </si>
+  <si>
+    <t>похороны</t>
+  </si>
+  <si>
+    <t>ДР</t>
+  </si>
+  <si>
+    <t>день рождения</t>
+  </si>
+  <si>
+    <t>помолвка</t>
+  </si>
+  <si>
+    <t>суд</t>
+  </si>
+  <si>
+    <t>прогулка</t>
+  </si>
+  <si>
+    <t>поход</t>
+  </si>
+  <si>
+    <t>вечеринка</t>
+  </si>
+  <si>
+    <t>пати</t>
+  </si>
+  <si>
+    <t>туса</t>
+  </si>
+  <si>
+    <t>дискотека</t>
+  </si>
+  <si>
+    <t>званый приём</t>
+  </si>
+  <si>
+    <t>вокзал</t>
+  </si>
+  <si>
+    <t>аэропорт</t>
+  </si>
+  <si>
+    <t>автовокзал</t>
+  </si>
+  <si>
+    <t>почта</t>
+  </si>
+  <si>
+    <t>рынок</t>
+  </si>
+  <si>
+    <t>фестиваль</t>
+  </si>
+  <si>
+    <t>конкурс</t>
+  </si>
+  <si>
+    <t>осмотр</t>
+  </si>
+  <si>
+    <t>проверка</t>
+  </si>
+  <si>
+    <t>проект</t>
+  </si>
+  <si>
+    <t>задание</t>
+  </si>
+  <si>
+    <t>план проекта</t>
+  </si>
+  <si>
+    <t>план</t>
+  </si>
+  <si>
     <t>Слово</t>
   </si>
   <si>
     <t>Теги</t>
   </si>
   <si>
-    <t>ребенок</t>
+    <t>диплом</t>
   </si>
   <si>
     <t>пробка</t>
   </si>
   <si>
-    <t>дети</t>
-  </si>
-  <si>
-    <t>noun_alt</t>
-  </si>
-  <si>
-    <t>to_be</t>
-  </si>
-  <si>
-    <t>дочь</t>
-  </si>
-  <si>
-    <t>move</t>
-  </si>
-  <si>
-    <t>сын</t>
-  </si>
-  <si>
-    <t>друг</t>
-  </si>
-  <si>
-    <t>remove</t>
-  </si>
-  <si>
-    <t>подруга</t>
-  </si>
-  <si>
-    <t>совещание</t>
-  </si>
-  <si>
-    <t>планерка</t>
-  </si>
-  <si>
-    <t>отец</t>
+    <t>уборка</t>
+  </si>
+  <si>
+    <t>картина</t>
+  </si>
+  <si>
+    <t>книга</t>
+  </si>
+  <si>
+    <t>гобелен</t>
   </si>
   <si>
     <t>аврал</t>
   </si>
   <si>
-    <t>мать</t>
-  </si>
-  <si>
-    <t>ремонт</t>
-  </si>
-  <si>
-    <t>квартира</t>
-  </si>
-  <si>
-    <t>place</t>
-  </si>
-  <si>
-    <t>автомастерская</t>
-  </si>
-  <si>
-    <t>дом</t>
-  </si>
-  <si>
-    <t>кухня</t>
-  </si>
-  <si>
-    <t>place_open</t>
-  </si>
-  <si>
-    <t>travel</t>
-  </si>
-  <si>
-    <t>ванная</t>
-  </si>
-  <si>
-    <t>goal</t>
+    <t>скульптура</t>
+  </si>
+  <si>
+    <t>мемуары</t>
+  </si>
+  <si>
+    <t>маникюр</t>
+  </si>
+  <si>
+    <t>педикюр</t>
+  </si>
+  <si>
+    <t>рейв</t>
+  </si>
+  <si>
+    <t>концерт</t>
+  </si>
+  <si>
+    <t>выставка</t>
+  </si>
+  <si>
+    <t>биеннале</t>
   </si>
   <si>
     <t>туалет</t>
   </si>
   <si>
-    <t>ноутбук</t>
-  </si>
-  <si>
-    <t>позаботиться</t>
-  </si>
-  <si>
-    <t>телефон</t>
-  </si>
-  <si>
-    <t>решить</t>
-  </si>
-  <si>
-    <t>смартфон</t>
-  </si>
-  <si>
-    <t>документы</t>
-  </si>
-  <si>
-    <t>тёща</t>
-  </si>
-  <si>
-    <t>project</t>
-  </si>
-  <si>
-    <t>тесть</t>
-  </si>
-  <si>
-    <t>курсы</t>
-  </si>
-  <si>
-    <t>свекровь</t>
-  </si>
-  <si>
-    <t>обучение</t>
-  </si>
-  <si>
-    <t>свёкр</t>
-  </si>
-  <si>
-    <t>ЖЭК</t>
-  </si>
-  <si>
-    <t>нотариус</t>
-  </si>
-  <si>
-    <t>бабушка</t>
-  </si>
-  <si>
-    <t>гипермаркет</t>
-  </si>
-  <si>
-    <t>дедушка</t>
-  </si>
-  <si>
-    <t>врач</t>
-  </si>
-  <si>
-    <t>доктор</t>
-  </si>
-  <si>
-    <t>дядя</t>
-  </si>
-  <si>
-    <t>тётя</t>
-  </si>
-  <si>
-    <t>ковёр</t>
-  </si>
-  <si>
-    <t>фикус</t>
-  </si>
-  <si>
-    <t>кактус</t>
-  </si>
-  <si>
-    <t>мебель</t>
-  </si>
-  <si>
-    <t>подумать</t>
-  </si>
-  <si>
-    <t>телек</t>
-  </si>
-  <si>
-    <t>убирать</t>
-  </si>
-  <si>
-    <t>ноут</t>
-  </si>
-  <si>
-    <t>добраться</t>
+    <t>галерея</t>
+  </si>
+  <si>
+    <t>музей</t>
+  </si>
+  <si>
+    <t>больница</t>
+  </si>
+  <si>
+    <t>поликлиника</t>
+  </si>
+  <si>
+    <t>курорт</t>
+  </si>
+  <si>
+    <t>отдых</t>
+  </si>
+  <si>
+    <t>санаторий</t>
+  </si>
+  <si>
+    <t>море</t>
+  </si>
+  <si>
+    <t>Чёрное море</t>
+  </si>
+  <si>
+    <t>Белое море</t>
+  </si>
+  <si>
+    <t>Красное море</t>
+  </si>
+  <si>
+    <t>Египет</t>
+  </si>
+  <si>
+    <t>Турция</t>
+  </si>
+  <si>
+    <t>Тайланд</t>
   </si>
   <si>
     <t>идти</t>
   </si>
   <si>
-    <t>выбраться</t>
-  </si>
-  <si>
     <t>ветеринар</t>
   </si>
   <si>
-    <t>зайти</t>
-  </si>
-  <si>
     <t>вернуть</t>
   </si>
   <si>
-    <t>забежать</t>
-  </si>
-  <si>
-    <t>съездить</t>
-  </si>
-  <si>
-    <t>поехать</t>
-  </si>
-  <si>
     <t>заняться</t>
-  </si>
-  <si>
-    <t>центр госуслуг</t>
-  </si>
-  <si>
-    <t>сгонять</t>
-  </si>
-  <si>
-    <t>родственники</t>
-  </si>
-  <si>
-    <t>дача</t>
-  </si>
-  <si>
-    <t>хранение</t>
-  </si>
-  <si>
-    <t>банк</t>
-  </si>
-  <si>
-    <t>свадьба</t>
-  </si>
-  <si>
-    <t>похороны</t>
-  </si>
-  <si>
-    <t>ДР</t>
-  </si>
-  <si>
-    <t>день рождения</t>
-  </si>
-  <si>
-    <t>помолвка</t>
-  </si>
-  <si>
-    <t>суд</t>
-  </si>
-  <si>
-    <t>прогулка</t>
-  </si>
-  <si>
-    <t>поход</t>
-  </si>
-  <si>
-    <t>вечеринка</t>
-  </si>
-  <si>
-    <t>пати</t>
-  </si>
-  <si>
-    <t>туса</t>
-  </si>
-  <si>
-    <t>дискотека</t>
-  </si>
-  <si>
-    <t>званый приём</t>
-  </si>
-  <si>
-    <t>вокзал</t>
-  </si>
-  <si>
-    <t>аэропорт</t>
-  </si>
-  <si>
-    <t>автовокзал</t>
-  </si>
-  <si>
-    <t>почта</t>
-  </si>
-  <si>
-    <t>рынок</t>
-  </si>
-  <si>
-    <t>фестиваль</t>
-  </si>
-  <si>
-    <t>конкурс</t>
-  </si>
-  <si>
-    <t>осмотр</t>
-  </si>
-  <si>
-    <t>проверка</t>
-  </si>
-  <si>
-    <t>проект</t>
-  </si>
-  <si>
-    <t>задание</t>
-  </si>
-  <si>
-    <t>план проекта</t>
-  </si>
-  <si>
-    <t>план</t>
-  </si>
-  <si>
-    <t>диплом</t>
-  </si>
-  <si>
-    <t>уборка</t>
-  </si>
-  <si>
-    <t>картина</t>
-  </si>
-  <si>
-    <t>книга</t>
-  </si>
-  <si>
-    <t>гобелен</t>
-  </si>
-  <si>
-    <t>скульптура</t>
-  </si>
-  <si>
-    <t>мемуары</t>
-  </si>
-  <si>
-    <t>маникюр</t>
-  </si>
-  <si>
-    <t>педикюр</t>
   </si>
 </sst>
 </file>
@@ -693,10 +777,10 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font/>
     <font>
       <b/>
     </font>
-    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -973,113 +1057,6 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="3.14"/>
-    <col customWidth="1" min="2" max="2" width="20.57"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2">
-        <v>2.0</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2">
-        <v>3.0</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2">
-        <v>4.0</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2">
-        <v>5.0</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2">
-        <v>7.0</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2">
-        <v>8.0</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2">
-        <v>9.0</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2">
-        <v>10.0</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="1" max="1" width="3.14"/>
     <col customWidth="1" min="2" max="2" width="8.57"/>
     <col customWidth="1" min="3" max="3" width="14.86"/>
     <col customWidth="1" min="4" max="4" width="16.29"/>
@@ -1090,7 +1067,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>5</v>
@@ -1104,13 +1081,13 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="C2" s="2">
         <v>1.0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3">
@@ -1118,13 +1095,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="C3" s="2">
         <v>1.0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>24</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4">
@@ -1132,13 +1109,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="C4" s="2">
         <v>1.0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5">
@@ -1146,13 +1123,13 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="C5" s="2">
         <v>1.0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6">
@@ -1160,13 +1137,13 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="C6" s="2">
         <v>1.0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7">
@@ -1174,13 +1151,13 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="C7" s="2">
         <v>1.0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8">
@@ -1188,13 +1165,13 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="C8" s="2">
         <v>1.0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9">
@@ -1202,13 +1179,13 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="C9" s="2">
         <v>1.0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10">
@@ -1216,13 +1193,13 @@
         <v>9.0</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="C10" s="2">
         <v>1.0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11">
@@ -1230,13 +1207,13 @@
         <v>10.0</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="C11" s="2">
         <v>1.0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12">
@@ -1244,13 +1221,13 @@
         <v>11.0</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="C12" s="2">
         <v>2.0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13">
@@ -1258,13 +1235,13 @@
         <v>12.0</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="C13" s="2">
         <v>2.0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14">
@@ -1272,13 +1249,13 @@
         <v>13.0</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="C14" s="2">
         <v>2.0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>47</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15">
@@ -1286,13 +1263,13 @@
         <v>14.0</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="C15" s="2">
         <v>2.0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16">
@@ -1300,13 +1277,13 @@
         <v>15.0</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="C16" s="2">
         <v>2.0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17">
@@ -1314,13 +1291,13 @@
         <v>16.0</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="C17" s="2">
         <v>2.0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18">
@@ -1328,13 +1305,13 @@
         <v>17.0</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="C18" s="2">
         <v>2.0</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19">
@@ -1342,13 +1319,13 @@
         <v>18.0</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="C19" s="2">
         <v>2.0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20">
@@ -1356,13 +1333,13 @@
         <v>19.0</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="C20" s="2">
         <v>2.0</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21">
@@ -1370,13 +1347,13 @@
         <v>20.0</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="C21" s="2">
         <v>2.0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22">
@@ -1384,13 +1361,13 @@
         <v>21.0</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="C22" s="2">
         <v>2.0</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23">
@@ -1398,13 +1375,13 @@
         <v>22.0</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="C23" s="2">
         <v>2.0</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24">
@@ -1412,13 +1389,13 @@
         <v>23.0</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="C24" s="2">
         <v>2.0</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25">
@@ -1426,13 +1403,13 @@
         <v>24.0</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="C25" s="2">
         <v>2.0</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26">
@@ -1440,13 +1417,13 @@
         <v>25.0</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="C26" s="2">
         <v>2.0</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1454,7 +1431,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -1482,7 +1459,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
@@ -1517,7 +1494,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C2" s="2">
         <v>1.0</v>
@@ -1538,7 +1515,7 @@
         <v>1.0</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3">
@@ -1567,7 +1544,7 @@
         <v>1.0</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4">
@@ -1575,7 +1552,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C4" s="2">
         <v>1.0</v>
@@ -1596,7 +1573,7 @@
         <v>1.0</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5">
@@ -1604,7 +1581,7 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C5" s="2">
         <v>1.0</v>
@@ -1625,7 +1602,7 @@
         <v>1.0</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6">
@@ -1633,7 +1610,7 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2">
         <v>1.0</v>
@@ -1654,7 +1631,7 @@
         <v>1.0</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7">
@@ -1662,7 +1639,7 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="C7" s="2">
         <v>1.0</v>
@@ -1683,7 +1660,7 @@
         <v>1.0</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8">
@@ -1691,7 +1668,7 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="C8" s="2">
         <v>1.0</v>
@@ -1712,7 +1689,7 @@
         <v>1.0</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9">
@@ -1720,7 +1697,7 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="C9" s="2">
         <v>1.0</v>
@@ -1741,7 +1718,7 @@
         <v>1.0</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10">
@@ -1749,7 +1726,7 @@
         <v>9.0</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="C10" s="2">
         <v>1.0</v>
@@ -1770,7 +1747,7 @@
         <v>1.0</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11">
@@ -1778,7 +1755,7 @@
         <v>10.0</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="C11" s="2">
         <v>1.0</v>
@@ -1797,7 +1774,7 @@
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12">
@@ -1805,7 +1782,7 @@
         <v>11.0</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="C12" s="2">
         <v>0.0</v>
@@ -1824,7 +1801,7 @@
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13">
@@ -1832,7 +1809,7 @@
         <v>12.0</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="C13" s="2">
         <v>0.0</v>
@@ -1851,7 +1828,7 @@
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14">
@@ -1859,7 +1836,7 @@
         <v>13.0</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="C14" s="2">
         <v>0.0</v>
@@ -1878,7 +1855,7 @@
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15">
@@ -1886,7 +1863,7 @@
         <v>14.0</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="C15" s="2">
         <v>1.0</v>
@@ -1905,7 +1882,7 @@
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16">
@@ -1913,7 +1890,7 @@
         <v>15.0</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="C16" s="2">
         <v>1.0</v>
@@ -1932,7 +1909,7 @@
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17">
@@ -1940,7 +1917,7 @@
         <v>16.0</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="C17" s="2">
         <v>0.0</v>
@@ -1959,7 +1936,7 @@
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18">
@@ -1967,7 +1944,7 @@
         <v>17.0</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="C18" s="2">
         <v>1.0</v>
@@ -1986,7 +1963,7 @@
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19">
@@ -1994,7 +1971,7 @@
         <v>18.0</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="C19" s="2">
         <v>1.0</v>
@@ -2013,7 +1990,7 @@
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20">
@@ -2021,7 +1998,7 @@
         <v>19.0</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="C20" s="2">
         <v>1.0</v>
@@ -2040,7 +2017,7 @@
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21">
@@ -2048,7 +2025,7 @@
         <v>20.0</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
       <c r="C21" s="2">
         <v>1.0</v>
@@ -2067,7 +2044,7 @@
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22">
@@ -2075,7 +2052,7 @@
         <v>21.0</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>78</v>
+        <v>45</v>
       </c>
       <c r="C22" s="2">
         <v>1.0</v>
@@ -2094,7 +2071,7 @@
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23">
@@ -2102,7 +2079,7 @@
         <v>22.0</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>80</v>
+        <v>46</v>
       </c>
       <c r="C23" s="2">
         <v>0.0</v>
@@ -2121,7 +2098,7 @@
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24">
@@ -2129,7 +2106,7 @@
         <v>23.0</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>84</v>
+        <v>47</v>
       </c>
       <c r="C24" s="2">
         <v>0.0</v>
@@ -2148,7 +2125,7 @@
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25">
@@ -2156,7 +2133,7 @@
         <v>24.0</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>86</v>
+        <v>48</v>
       </c>
       <c r="C25" s="2">
         <v>0.0</v>
@@ -2175,7 +2152,7 @@
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26">
@@ -2183,7 +2160,7 @@
         <v>25.0</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="C26" s="2">
         <v>1.0</v>
@@ -2202,7 +2179,7 @@
       </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27">
@@ -2210,7 +2187,7 @@
         <v>26.0</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="C27" s="2">
         <v>1.0</v>
@@ -2229,7 +2206,7 @@
       </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28">
@@ -2237,7 +2214,7 @@
         <v>27.0</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="C28" s="2">
         <v>1.0</v>
@@ -2256,7 +2233,7 @@
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29">
@@ -2264,7 +2241,7 @@
         <v>28.0</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>90</v>
+        <v>54</v>
       </c>
       <c r="C29" s="2">
         <v>1.0</v>
@@ -2283,7 +2260,7 @@
       </c>
       <c r="H29" s="2"/>
       <c r="I29" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30">
@@ -2291,7 +2268,7 @@
         <v>29.0</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>91</v>
+        <v>56</v>
       </c>
       <c r="C30" s="2">
         <v>1.0</v>
@@ -2310,7 +2287,7 @@
       </c>
       <c r="H30" s="2"/>
       <c r="I30" s="2" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31">
@@ -2318,7 +2295,7 @@
         <v>30.0</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>92</v>
+        <v>59</v>
       </c>
       <c r="C31" s="2">
         <v>0.0</v>
@@ -2336,7 +2313,78 @@
         <v>0.0</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -2359,7 +2407,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2">
@@ -2367,7 +2415,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3">
@@ -2375,7 +2423,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4">
@@ -2383,31 +2431,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2">
-        <v>4.0</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2">
-        <v>5.0</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -2418,19 +2442,30 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
+    <tabColor rgb="FFFFE599"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="3.14"/>
+    <col customWidth="1" min="2" max="2" width="20.57"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>93</v>
+        <v>86</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="2">
@@ -2438,7 +2473,13 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="3">
@@ -2446,7 +2487,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="4">
@@ -2454,7 +2501,155 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>96</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2">
+        <v>9.0</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2">
+        <v>10.0</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2477,7 +2672,7 @@
     <col customWidth="1" min="2" max="2" width="15.0"/>
     <col customWidth="1" min="3" max="3" width="3.86"/>
     <col customWidth="1" min="4" max="4" width="6.29"/>
-    <col customWidth="1" min="5" max="5" width="6.86"/>
+    <col customWidth="1" min="5" max="5" width="10.71"/>
     <col customWidth="1" min="6" max="7" width="15.14"/>
   </cols>
   <sheetData>
@@ -2486,27 +2681,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F1" s="3" t="s">
         <v>101</v>
       </c>
+      <c r="F1" s="4" t="s">
+        <v>103</v>
+      </c>
       <c r="G1" s="1" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2">
       <c r="B2" s="2" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="C2" s="2">
         <v>1.0</v>
@@ -2515,95 +2710,95 @@
         <v>1.0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" s="2" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="2" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="2" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="2" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="2" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="2" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="2" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14">
@@ -2611,47 +2806,47 @@
         <v>130</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="3" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17">
-      <c r="B17" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>128</v>
+      <c r="B17" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20">
@@ -2659,7 +2854,7 @@
         <v>141</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21">
@@ -2667,7 +2862,7 @@
         <v>142</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22">
@@ -2675,7 +2870,7 @@
         <v>143</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23">
@@ -2683,116 +2878,116 @@
         <v>145</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" s="2" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" s="2" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" s="2" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" s="2" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" s="2" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" s="2" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
     </row>
     <row r="34">
       <c r="B34" s="2" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35">
       <c r="B35" s="2" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36">
       <c r="B36" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="37">
       <c r="B37" s="2" t="s">
-        <v>126</v>
+        <v>163</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>8</v>
@@ -2800,7 +2995,7 @@
     </row>
     <row r="38">
       <c r="B38" s="2" t="s">
-        <v>148</v>
+        <v>165</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>8</v>
@@ -2808,55 +3003,55 @@
     </row>
     <row r="39">
       <c r="B39" s="2" t="s">
-        <v>153</v>
+        <v>166</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" s="2" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" s="2" t="s">
-        <v>151</v>
+        <v>170</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42">
       <c r="B42" s="2" t="s">
-        <v>155</v>
+        <v>172</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
     </row>
     <row r="43">
       <c r="B43" s="2" t="s">
-        <v>156</v>
+        <v>173</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
     </row>
     <row r="44">
       <c r="B44" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="45">
       <c r="B45" s="2" t="s">
-        <v>146</v>
+        <v>176</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>8</v>
@@ -2864,7 +3059,7 @@
     </row>
     <row r="46">
       <c r="B46" s="2" t="s">
-        <v>121</v>
+        <v>177</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>8</v>
@@ -2872,26 +3067,26 @@
     </row>
     <row r="47">
       <c r="B47" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
     </row>
     <row r="48">
       <c r="B48" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E48" s="4" t="s">
+      <c r="E48" s="3" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="49">
       <c r="B49" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="50">
@@ -2907,12 +3102,12 @@
         <v>182</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="52">
       <c r="B52" s="2" t="s">
-        <v>122</v>
+        <v>183</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>8</v>
@@ -2920,7 +3115,7 @@
     </row>
     <row r="53">
       <c r="B53" s="2" t="s">
-        <v>146</v>
+        <v>176</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>8</v>
@@ -2928,7 +3123,7 @@
     </row>
     <row r="54">
       <c r="B54" s="2" t="s">
-        <v>148</v>
+        <v>165</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>8</v>
@@ -2936,7 +3131,7 @@
     </row>
     <row r="55">
       <c r="B55" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>8</v>
@@ -2944,7 +3139,7 @@
     </row>
     <row r="56">
       <c r="B56" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>8</v>
@@ -2952,7 +3147,7 @@
     </row>
     <row r="57">
       <c r="B57" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>8</v>
@@ -2960,7 +3155,7 @@
     </row>
     <row r="58">
       <c r="B58" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>8</v>
@@ -2968,7 +3163,7 @@
     </row>
     <row r="59">
       <c r="B59" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>8</v>
@@ -2976,15 +3171,15 @@
     </row>
     <row r="60">
       <c r="B60" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="61">
       <c r="B61" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>8</v>
@@ -2992,15 +3187,15 @@
     </row>
     <row r="62">
       <c r="B62" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>8</v>
+        <v>191</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="63">
       <c r="B63" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>8</v>
@@ -3008,7 +3203,7 @@
     </row>
     <row r="64">
       <c r="B64" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>8</v>
@@ -3016,7 +3211,7 @@
     </row>
     <row r="65">
       <c r="B65" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>8</v>
@@ -3024,7 +3219,7 @@
     </row>
     <row r="66">
       <c r="B66" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>8</v>
@@ -3032,7 +3227,7 @@
     </row>
     <row r="67">
       <c r="B67" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>8</v>
@@ -3040,63 +3235,63 @@
     </row>
     <row r="68">
       <c r="B68" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="E68" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="E68" s="3" t="s">
         <v>132</v>
       </c>
       <c r="F68" s="2"/>
       <c r="G68" s="2" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
     </row>
     <row r="69">
       <c r="B69" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="70">
       <c r="B70" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="E70" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="E70" s="3" t="s">
         <v>132</v>
       </c>
       <c r="F70" s="2"/>
       <c r="G70" s="2" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
     </row>
     <row r="71">
       <c r="B71" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="E71" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="E71" s="3" t="s">
         <v>132</v>
       </c>
       <c r="F71" s="2"/>
       <c r="G71" s="2" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
     </row>
     <row r="72">
       <c r="B72" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="E72" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="E72" s="3" t="s">
         <v>132</v>
       </c>
       <c r="F72" s="2"/>
       <c r="G72" s="2" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
     </row>
     <row r="73">
       <c r="B73" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>8</v>
@@ -3104,7 +3299,7 @@
     </row>
     <row r="74">
       <c r="B74" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>8</v>
@@ -3112,7 +3307,7 @@
     </row>
     <row r="75">
       <c r="B75" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>8</v>
@@ -3120,7 +3315,7 @@
     </row>
     <row r="76">
       <c r="B76" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>8</v>
@@ -3128,71 +3323,80 @@
     </row>
     <row r="77">
       <c r="B77" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E77" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E77" s="3" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="78">
       <c r="B78" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="E78" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="E78" s="3" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="79">
       <c r="B79" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="E79" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E79" s="3" t="s">
         <v>144</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="80">
       <c r="B80" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E80" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="E80" s="3" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="81">
       <c r="B81" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="E81" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="E81" s="3" t="s">
         <v>144</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="82">
       <c r="B82" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="E82" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E82" s="3" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="83">
       <c r="B83" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="E83" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="E83" s="3" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="84">
       <c r="B84" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="E84" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="E84" s="3" t="s">
         <v>144</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="85">
       <c r="B85" s="2" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>144</v>
@@ -3200,39 +3404,51 @@
     </row>
     <row r="86">
       <c r="B86" s="2" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>144</v>
       </c>
+      <c r="F86" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="87">
       <c r="B87" s="2" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>144</v>
       </c>
+      <c r="F87" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="88">
       <c r="B88" s="2" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>144</v>
       </c>
+      <c r="F88" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="89">
       <c r="B89" s="2" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>144</v>
       </c>
+      <c r="F89" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="90">
       <c r="B90" s="2" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>144</v>
@@ -3240,18 +3456,162 @@
     </row>
     <row r="91">
       <c r="B91" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="E91" s="2" t="s">
-        <v>144</v>
+        <v>221</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="92">
       <c r="B92" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="E92" s="2" t="s">
-        <v>144</v>
+        <v>222</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="B93" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="B94" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="B95" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="B96" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="B97" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="B98" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="B99" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="B100" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="B101" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="B102" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="B103" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="B104" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="B105" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="B106" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="B107" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="B108" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="B109" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="B110" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -3272,6 +3632,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="3.14"/>
     <col customWidth="1" min="2" max="2" width="17.14"/>
+    <col customWidth="1" min="4" max="4" width="8.14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3279,22 +3640,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>113</v>
+        <v>103</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>109</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2">
@@ -3302,13 +3663,13 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3">
@@ -3319,10 +3680,10 @@
         <v>23</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4">
@@ -3330,16 +3691,16 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5">
@@ -3347,13 +3708,13 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6">
@@ -3361,13 +3722,13 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7">
@@ -3375,13 +3736,13 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8">
@@ -3389,13 +3750,13 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9">
@@ -3403,13 +3764,13 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10">
@@ -3417,13 +3778,13 @@
         <v>9.0</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11">
@@ -3431,16 +3792,16 @@
         <v>10.0</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12">
@@ -3448,16 +3809,16 @@
         <v>11.0</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>133</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13">
@@ -3465,13 +3826,13 @@
         <v>12.0</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14">
@@ -3479,16 +3840,16 @@
         <v>13.0</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>133</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15">
@@ -3496,13 +3857,16 @@
         <v>14.0</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>104</v>
+        <v>134</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="16">
@@ -3510,16 +3874,16 @@
         <v>15.0</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17">
@@ -3527,13 +3891,13 @@
         <v>16.0</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>133</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18">
@@ -3541,13 +3905,13 @@
         <v>17.0</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19">
@@ -3555,10 +3919,10 @@
         <v>18.0</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>144</v>
@@ -3569,13 +3933,13 @@
         <v>19.0</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21">
@@ -3583,10 +3947,10 @@
         <v>20.0</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>144</v>
@@ -3597,10 +3961,10 @@
         <v>21.0</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>78</v>
+        <v>45</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>144</v>
@@ -3611,10 +3975,10 @@
         <v>22.0</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>80</v>
+        <v>46</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>144</v>
@@ -3625,10 +3989,10 @@
         <v>23.0</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>84</v>
+        <v>47</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>144</v>
@@ -3639,10 +4003,10 @@
         <v>24.0</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>86</v>
+        <v>48</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>144</v>
@@ -3653,16 +4017,16 @@
         <v>25.0</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27">
@@ -3670,13 +4034,13 @@
         <v>26.0</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28">
@@ -3684,13 +4048,13 @@
         <v>27.0</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29">
@@ -3698,10 +4062,10 @@
         <v>28.0</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>90</v>
+        <v>54</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>144</v>
@@ -3715,10 +4079,10 @@
         <v>29.0</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>144</v>
@@ -3732,13 +4096,13 @@
         <v>30.0</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="32">
@@ -3746,15 +4110,15 @@
         <v>31.0</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>133</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="F32" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F32" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3763,13 +4127,13 @@
         <v>32.0</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>133</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>8</v>
@@ -3780,13 +4144,13 @@
         <v>33.0</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>133</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="35">
@@ -3794,13 +4158,13 @@
         <v>34.0</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>133</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="36">
@@ -3808,13 +4172,13 @@
         <v>35.0</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>133</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="37">
@@ -3822,13 +4186,13 @@
         <v>36.0</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>133</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>8</v>
@@ -3839,13 +4203,13 @@
         <v>37.0</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>133</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>8</v>
@@ -3856,13 +4220,13 @@
         <v>38.0</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>133</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40">
@@ -3870,13 +4234,13 @@
         <v>39.0</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>133</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -3899,105 +4263,105 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>108</v>
+        <v>210</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>109</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>111</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>121</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>122</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>124</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>126</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>129</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="21">
@@ -4012,22 +4376,22 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>136</v>
+        <v>227</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="27">
@@ -4037,37 +4401,37 @@
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>146</v>
+        <v>176</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
-        <v>148</v>
+        <v>165</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="s">
-        <v>151</v>
+        <v>170</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">
-        <v>153</v>
+        <v>166</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="s">
-        <v>155</v>
+        <v>172</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="s">
-        <v>156</v>
+        <v>173</v>
       </c>
     </row>
     <row r="35">
@@ -4082,47 +4446,47 @@
     </row>
     <row r="37">
       <c r="A37" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="46">
@@ -4132,52 +4496,52 @@
     </row>
     <row r="47">
       <c r="A47" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="s">
-        <v>168</v>
+        <v>242</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="s">
-        <v>170</v>
+        <v>243</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="s">
-        <v>172</v>
+        <v>244</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="s">
-        <v>176</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>